<commit_message>
Reformatted Sprint 2 Test Cases
</commit_message>
<xml_diff>
--- a/Documents/Sprint 2/Sprint 2 Test Cases.xlsx
+++ b/Documents/Sprint 2/Sprint 2 Test Cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ymens\Desktop\Pace Classes\CS 691 Capstone (FitForce)\Sprint 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egasa\OneDrive\Desktop\School\CS 691 CS Capstone\Sprint 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30A6C3E-419C-4E11-BB84-B000220EF45C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D219D70-23FD-4391-9445-E8A9C987FD62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{39305A45-FD0E-4755-B779-09F504698BBA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{39305A45-FD0E-4755-B779-09F504698BBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -664,21 +664,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35849A8B-717D-467A-8366-A9D67EA0751B}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="G1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="26.109375" customWidth="1"/>
-    <col min="3" max="3" width="39.5546875" customWidth="1"/>
-    <col min="4" max="4" width="26.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="34" customWidth="1"/>
+    <col min="2" max="2" width="26.08984375" customWidth="1"/>
+    <col min="3" max="3" width="37.1796875" customWidth="1"/>
+    <col min="4" max="4" width="26.08984375" customWidth="1"/>
+    <col min="5" max="5" width="7.7265625" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" customWidth="1"/>
+    <col min="7" max="7" width="7.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="9" customFormat="1" ht="15.6">
+    <row r="1" spans="1:7" s="9" customFormat="1" ht="16">
       <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
@@ -689,7 +689,7 @@
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" ht="23.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -712,7 +712,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="55.2">
+    <row r="3" spans="1:7" ht="52">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -744,7 +744,7 @@
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:7" s="9" customFormat="1" ht="15.6">
+    <row r="5" spans="1:7" s="9" customFormat="1" ht="16">
       <c r="A5" s="11" t="s">
         <v>14</v>
       </c>
@@ -755,7 +755,7 @@
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" ht="24" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -778,7 +778,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="41.4">
+    <row r="7" spans="1:7" ht="39">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -801,7 +801,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="41.4">
+    <row r="8" spans="1:7" ht="39">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -824,7 +824,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="9" customFormat="1" ht="15.6">
+    <row r="10" spans="1:7" s="9" customFormat="1" ht="16">
       <c r="A10" s="10" t="s">
         <v>17</v>
       </c>
@@ -835,7 +835,7 @@
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" ht="26" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -858,7 +858,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="55.2">
+    <row r="12" spans="1:7" ht="52">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -890,7 +890,7 @@
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:7" s="9" customFormat="1" ht="15.6">
+    <row r="14" spans="1:7" s="9" customFormat="1" ht="16">
       <c r="A14" s="11" t="s">
         <v>19</v>
       </c>
@@ -901,7 +901,7 @@
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" ht="25.5" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -924,7 +924,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="55.2">
+    <row r="16" spans="1:7" ht="52">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -947,7 +947,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="9" customFormat="1" ht="15.6">
+    <row r="18" spans="1:7" s="9" customFormat="1" ht="16">
       <c r="A18" s="10" t="s">
         <v>21</v>
       </c>
@@ -958,7 +958,7 @@
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" ht="23" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -981,7 +981,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="69">
+    <row r="20" spans="1:7" ht="52">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -1013,7 +1013,7 @@
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="1:7" s="9" customFormat="1" ht="15.6">
+    <row r="22" spans="1:7" s="9" customFormat="1" ht="16">
       <c r="A22" s="11" t="s">
         <v>23</v>
       </c>
@@ -1024,7 +1024,7 @@
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" ht="27.5" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="55.2">
+    <row r="24" spans="1:7" ht="52">
       <c r="A24" s="2" t="s">
         <v>24</v>
       </c>
@@ -1080,5 +1080,6 @@
     <mergeCell ref="A10:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>